<commit_message>
[KhoaNguyen] Update todo list
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\ExternalProject\Nail\Source\ShopNail_Ver1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>MainActivity</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>- Show data</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In-progress</t>
   </si>
 </sst>
 </file>
@@ -118,18 +124,18 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,12 +420,13 @@
   <dimension ref="B3:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
@@ -428,252 +435,242 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="2"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="2"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="2"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="2"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="2"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="2"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="B25:B27"/>
@@ -690,7 +687,21 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>